<commit_message>
fixed it i hope
</commit_message>
<xml_diff>
--- a/starting_rotation/data/raw/archive/first_lineup.xlsx
+++ b/starting_rotation/data/raw/archive/first_lineup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Documents\School\University of Texas-Austin\Classes\Data Mining\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidscolari/Dropbox/grad_school/3_Spring22/data_mining_final/starting_rotation/data/raw/archive/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3EA6DF88-BA45-42C2-8B07-47782D98361C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D844BE-69E5-0249-906E-25BA5BF88E46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="first_lineup" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
   <si>
     <t>id</t>
   </si>
@@ -194,12 +194,6 @@
   </si>
   <si>
     <t>Sale</t>
-  </si>
-  <si>
-    <t>Chad</t>
-  </si>
-  <si>
-    <t>Bettis</t>
   </si>
   <si>
     <t>Yu</t>
@@ -211,8 +205,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,6 +340,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -689,8 +689,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1045,14 +1046,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1063,7 +1066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>572096</v>
       </c>
@@ -1074,7 +1077,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>433587</v>
       </c>
@@ -1085,7 +1088,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>502042</v>
       </c>
@@ -1096,7 +1099,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>502154</v>
       </c>
@@ -1107,7 +1110,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>451584</v>
       </c>
@@ -1118,7 +1121,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>572971</v>
       </c>
@@ -1129,7 +1132,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>446372</v>
       </c>
@@ -1140,7 +1143,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>502381</v>
       </c>
@@ -1151,7 +1154,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>456034</v>
       </c>
@@ -1162,7 +1165,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>453286</v>
       </c>
@@ -1173,7 +1176,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>547973</v>
       </c>
@@ -1184,7 +1187,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>477132</v>
       </c>
@@ -1195,7 +1198,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>518516</v>
       </c>
@@ -1206,7 +1209,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>543243</v>
       </c>
@@ -1217,7 +1220,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>434718</v>
       </c>
@@ -1228,7 +1231,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>502202</v>
       </c>
@@ -1239,7 +1242,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>425844</v>
       </c>
@@ -1250,7 +1253,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>474521</v>
       </c>
@@ -1261,7 +1264,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>519455</v>
       </c>
@@ -1272,7 +1275,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>594798</v>
       </c>
@@ -1283,7 +1286,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>543037</v>
       </c>
@@ -1294,7 +1297,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>453343</v>
       </c>
@@ -1305,7 +1308,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>453562</v>
       </c>
@@ -1316,7 +1319,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>453192</v>
       </c>
@@ -1327,7 +1330,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3">
       <c r="A26">
         <v>544931</v>
       </c>
@@ -1338,7 +1341,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3">
       <c r="A27">
         <v>543521</v>
       </c>
@@ -1349,7 +1352,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3">
       <c r="A28">
         <v>608379</v>
       </c>
@@ -1360,7 +1363,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3">
       <c r="A29">
         <v>519242</v>
       </c>
@@ -1371,26 +1374,26 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30">
-        <v>518452</v>
-      </c>
-      <c r="B30" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3">
+      <c r="A30" s="1">
+        <v>425844</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31">
         <v>506433</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>